<commit_message>
Final Test Case Added
</commit_message>
<xml_diff>
--- a/Search Feature Test Case.xlsx
+++ b/Search Feature Test Case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7500"/>
+    <workbookView windowWidth="20490" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>TEST CASE ID</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t xml:space="preserve">Varify Search Using  name, brand, category, color, size, or SKU </t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>Chrome ,Mozila</t>
   </si>
   <si>
     <t>Application is running, search bar is available, and products with all relevant attributes exist in the system</t>
@@ -139,6 +145,9 @@
   </si>
   <si>
     <t>Varify The out of stock Product</t>
+  </si>
+  <si>
+    <t>p4</t>
   </si>
   <si>
     <t xml:space="preserve">01.Enter e out of stock product
@@ -186,6 +195,9 @@
   </si>
   <si>
     <t>Varify The Voice or text Search</t>
+  </si>
+  <si>
+    <t>p2</t>
   </si>
   <si>
     <t>Use voice input or text input</t>
@@ -242,7 +254,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,13 +281,6 @@
       <color rgb="FF3A3A3A"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -731,152 +736,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -886,9 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1223,8 +1225,8 @@
   <sheetPr/>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1232,7 +1234,7 @@
     <col min="1" max="1" width="19.8571428571429" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.7142857142857" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.4285714285714" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5714285714286" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5714285714286" style="3" customWidth="1"/>
     <col min="5" max="5" width="43.2857142857143" style="3" customWidth="1"/>
     <col min="6" max="6" width="23.8571428571429" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.8571428571429" style="3" customWidth="1"/>
@@ -1242,34 +1244,34 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="29" customHeight="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1280,221 +1282,308 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" ht="45" spans="1:10">
       <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="5" ht="30" spans="1:10">
+    <row r="5" ht="45" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>23</v>
+      <c r="I5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" ht="60" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="9" ht="30" spans="1:10">
+    <row r="9" ht="45" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" ht="45" spans="1:10">
       <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>54</v>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="45" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="J11" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>